<commit_message>
The dichroic curves were added to the code
</commit_message>
<xml_diff>
--- a/AIS/SPARC4_Spectral_Response/Channel 0/ccd.xlsx
+++ b/AIS/SPARC4_Spectral_Response/Channel 0/ccd.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Wavelength</t>
   </si>
@@ -37,49 +37,97 @@
     <t xml:space="preserve">350.0</t>
   </si>
   <si>
+    <t xml:space="preserve">38.43</t>
+  </si>
+  <si>
     <t xml:space="preserve">400.0</t>
   </si>
   <si>
+    <t xml:space="preserve">85.39</t>
+  </si>
+  <si>
     <t xml:space="preserve">450.0</t>
   </si>
   <si>
+    <t xml:space="preserve">86.86</t>
+  </si>
+  <si>
     <t xml:space="preserve">500.0</t>
   </si>
   <si>
+    <t xml:space="preserve">85.12</t>
+  </si>
+  <si>
     <t xml:space="preserve">550.0</t>
   </si>
   <si>
+    <t xml:space="preserve">88.96</t>
+  </si>
+  <si>
     <t xml:space="preserve">600.0</t>
   </si>
   <si>
+    <t xml:space="preserve">89.12</t>
+  </si>
+  <si>
     <t xml:space="preserve">650.0</t>
   </si>
   <si>
+    <t xml:space="preserve">87.01</t>
+  </si>
+  <si>
     <t xml:space="preserve">700.0</t>
   </si>
   <si>
+    <t xml:space="preserve">84.12</t>
+  </si>
+  <si>
     <t xml:space="preserve">750.0</t>
   </si>
   <si>
+    <t xml:space="preserve">73.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">800.0</t>
   </si>
   <si>
+    <t xml:space="preserve">61.44</t>
+  </si>
+  <si>
     <t xml:space="preserve">850.0</t>
   </si>
   <si>
+    <t xml:space="preserve">44.32</t>
+  </si>
+  <si>
     <t xml:space="preserve">900.0</t>
   </si>
   <si>
+    <t xml:space="preserve">30.32</t>
+  </si>
+  <si>
     <t xml:space="preserve">950.0</t>
   </si>
   <si>
+    <t xml:space="preserve">16.49</t>
+  </si>
+  <si>
     <t xml:space="preserve">1000.0</t>
   </si>
   <si>
+    <t xml:space="preserve">5.67</t>
+  </si>
+  <si>
     <t xml:space="preserve">1050.0</t>
   </si>
   <si>
+    <t xml:space="preserve">1.56</t>
+  </si>
+  <si>
     <t xml:space="preserve">1100.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.35</t>
   </si>
 </sst>
 </file>
@@ -212,7 +260,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.68359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -244,134 +292,134 @@
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="n">
-        <v>100</v>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>100</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>100</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>100</v>
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>100</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>100</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <v>100</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>100</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <v>100</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5" t="n">
-        <v>100</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="n">
-        <v>100</v>
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>100</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="5" t="n">
-        <v>100</v>
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5" t="n">
-        <v>100</v>
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>